<commit_message>
updated unit test cases
</commit_message>
<xml_diff>
--- a/testfiles/1.1 - Audacy Zero - Procedure Example.xlsx
+++ b/testfiles/1.1 - Audacy Zero - Procedure Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarunigattu/repositories/quantum/testfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE90F6B5-CA68-BB42-872A-688E8BEDAA9B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D54C45-E6F4-A944-9E7A-7941AE6C9A99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,6 +435,60 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B87638F5-C2DE-EE41-BD90-1551EEB255D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -737,7 +791,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -974,7 +1030,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>32</v>
@@ -1069,7 +1125,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>46</v>

</xml_diff>